<commit_message>
Tweak export_models template interface to support IC QC reference files
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_ic_reference_all_non_res_land_details.xlsx
+++ b/dbt/export/templates/qc.vw_ic_reference_all_non_res_land_details.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2532CA20-CE62-47C3-8B99-1A041E64BA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1842C7F7-D5C9-4202-97CB-79CDFA8E080B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Query Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>

<commit_message>
Make sheet name configurable in `export_models` and use it to tweak sheet name for IC reference files
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_ic_reference_all_non_res_land_details.xlsx
+++ b/dbt/export/templates/qc.vw_ic_reference_all_non_res_land_details.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\ic_reference_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1842C7F7-D5C9-4202-97CB-79CDFA8E080B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8486AD18-01AC-4EBC-A245-C5EE5F785EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Query Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>

<commit_message>
Update IC reference files to match format for missing data and sheet names with Inquire (#709)
* Allow QC exports to format blank cells as empty strings

* Move model export log to after we write the Excel file

* Make sheet name configurable in `export_models` and use it to tweak sheet name for IC reference files

* Use YAML anchors/aliases to centralize format_blanks_as_empty_string configs in QC exports
</commit_message>
<xml_diff>
--- a/dbt/export/templates/qc.vw_ic_reference_all_non_res_land_details.xlsx
+++ b/dbt/export/templates/qc.vw_ic_reference_all_non_res_land_details.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jecochr\Downloads\ic_reference_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1842C7F7-D5C9-4202-97CB-79CDFA8E080B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8486AD18-01AC-4EBC-A245-C5EE5F785EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Query Results" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>